<commit_message>
V0.1.4 - Neue Struktur mit Mapper, Wrapper und Control
</commit_message>
<xml_diff>
--- a/documentation/ESP32/Pinout.xlsx
+++ b/documentation/ESP32/Pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projekte\LandRover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roberttrampler/Projekte/LandRover/GIT_LandRover/LandRover_ESP32/documentation/ESP32/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39AEAB40-FF24-459C-B1C3-10DC4040E235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9EB0264-D682-CD47-AAD6-10D09DA28409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{1CF20767-7363-42F2-8642-5539791B45CC}"/>
+    <workbookView xWindow="9720" yWindow="660" windowWidth="18960" windowHeight="19080" activeTab="1" xr2:uid="{1CF20767-7363-42F2-8642-5539791B45CC}"/>
   </bookViews>
   <sheets>
     <sheet name="DOIT ESP32 DEVKIT V1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="211">
   <si>
     <t>pin1</t>
   </si>
@@ -697,6 +697,24 @@
   </si>
   <si>
     <t>Manche Widerstände an den Ausgängen fehlen hier noch. Zum Beispiel Dummy</t>
+  </si>
+  <si>
+    <t>CH2 Transmission</t>
+  </si>
+  <si>
+    <t>Shaker</t>
+  </si>
+  <si>
+    <t>Position lights</t>
+  </si>
+  <si>
+    <t>Blink  lights right</t>
+  </si>
+  <si>
+    <t>Blink lights left</t>
+  </si>
+  <si>
+    <t>Rear / Brake lights</t>
   </si>
 </sst>
 </file>
@@ -1589,23 +1607,23 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.54296875" customWidth="1"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.81640625" customWidth="1"/>
-    <col min="8" max="8" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="1.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2" customWidth="1"/>
-    <col min="11" max="11" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.6328125" customWidth="1"/>
-    <col min="14" max="14" width="11.36328125" customWidth="1"/>
-    <col min="15" max="15" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" customWidth="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2" customWidth="1"/>
-    <col min="17" max="17" width="7.1796875" customWidth="1"/>
-    <col min="18" max="18" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.1640625" customWidth="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:18">
@@ -2346,27 +2364,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245388F8-018A-4F5D-BD5E-A891996E22D8}">
   <dimension ref="B3:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="107" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.54296875" customWidth="1"/>
-    <col min="4" max="4" width="1.7265625" customWidth="1"/>
-    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.81640625" customWidth="1"/>
-    <col min="8" max="8" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="1.6640625" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="2" customWidth="1"/>
-    <col min="11" max="11" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="4.6328125" customWidth="1"/>
-    <col min="14" max="14" width="11.36328125" customWidth="1"/>
-    <col min="15" max="15" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" customWidth="1"/>
+    <col min="14" max="14" width="11.33203125" customWidth="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="2" customWidth="1"/>
-    <col min="17" max="17" width="7.1796875" customWidth="1"/>
-    <col min="18" max="18" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.1640625" customWidth="1"/>
+    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:18">
@@ -2457,7 +2475,7 @@
         <v>104</v>
       </c>
       <c r="O8" s="13" t="s">
-        <v>81</v>
+        <v>206</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>97</v>
@@ -2744,7 +2762,7 @@
         <v>107</v>
       </c>
       <c r="O15" s="14" t="s">
-        <v>110</v>
+        <v>207</v>
       </c>
       <c r="Q15" s="3" t="s">
         <v>99</v>
@@ -2789,7 +2807,7 @@
         <v>104</v>
       </c>
       <c r="O16" s="14" t="s">
-        <v>83</v>
+        <v>208</v>
       </c>
       <c r="Q16" s="3" t="s">
         <v>99</v>
@@ -2894,7 +2912,7 @@
         <v>97</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>79</v>
+        <v>205</v>
       </c>
       <c r="F19" s="20" t="s">
         <v>104</v>
@@ -2922,7 +2940,7 @@
         <v>104</v>
       </c>
       <c r="O19" s="14" t="s">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="Q19" s="3" t="s">
         <v>99</v>
@@ -3035,7 +3053,7 @@
         <v>104</v>
       </c>
       <c r="O22" s="14" t="s">
-        <v>82</v>
+        <v>209</v>
       </c>
       <c r="Q22" s="3" t="s">
         <v>99</v>
@@ -3225,7 +3243,7 @@
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3240,15 +3258,15 @@
       <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.453125" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="79.36328125" style="30" customWidth="1"/>
+    <col min="1" max="1" width="24.5" style="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="79.33203125" style="30" customWidth="1"/>
     <col min="3" max="3" width="5" style="30" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.81640625" style="30" customWidth="1"/>
-    <col min="5" max="5" width="25.6328125" style="30" customWidth="1"/>
-    <col min="6" max="6" width="25.36328125" style="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.81640625" style="30"/>
+    <col min="4" max="4" width="25.83203125" style="30" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" style="30" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" style="30" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="30"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3394,7 +3412,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="16.5">
+    <row r="11" spans="1:6" ht="18">
       <c r="A11" s="3" t="s">
         <v>175</v>
       </c>
@@ -3678,7 +3696,7 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>